<commit_message>
Better Architect Menu - 3563882422 업데이트
</commit_message>
<xml_diff>
--- a/Data/ferny/Better Architect Menu - 3563882422/Better Architect Menu - 3563882422.xlsx
+++ b/Data/ferny/Better Architect Menu - 3563882422/Better Architect Menu - 3563882422.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Better Architect Menu - 3563882422\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD890B8-9FA4-4412-B809-ED3CE587EB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD72DE6-13DA-40A1-832A-BC04BFBB15E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="889">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1185" uniqueCount="916">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -448,9 +448,6 @@
     <t>DesignationCategoryDef+Ferny_ProductionInfrastructure.label</t>
   </si>
   <si>
-    <t>Infrastructure</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -463,7 +460,7 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>DesignationCategoryDef+Ferny_ProductionInfrastructure.description</t>
+    <t>Infrastructure</t>
   </si>
   <si>
     <r>
@@ -478,13 +475,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_ProductionInfrastructure.description</t>
+  </si>
+  <si>
     <t>Ferny_ProductionInfrastructure.description</t>
   </si>
   <si>
     <t>Managing production.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_PowerGeneration.label</t>
   </si>
   <si>
     <r>
@@ -499,6 +496,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_PowerGeneration.label</t>
+  </si>
+  <si>
     <t>Ferny_PowerGeneration.label</t>
   </si>
   <si>
@@ -568,9 +568,6 @@
     <t>Ferny_PowerManagement.label</t>
   </si>
   <si>
-    <t>DesignationCategoryDef+Ferny_PowerManagement.description</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -583,13 +580,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_PowerManagement.description</t>
+  </si>
+  <si>
     <t>Ferny_PowerManagement.description</t>
   </si>
   <si>
     <t>Things that help you manage your power.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Animals.label</t>
   </si>
   <si>
     <r>
@@ -604,6 +601,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Animals.label</t>
+  </si>
+  <si>
     <t>Ferny_Animals.label</t>
   </si>
   <si>
@@ -811,13 +811,10 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_CombatInfrastructure.description</t>
+  </si>
+  <si>
     <t>Ferny_CombatInfrastructure.description</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_CombatInfrastructure.description</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Ranching.label</t>
   </si>
   <si>
     <r>
@@ -844,10 +841,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Ranching.label</t>
+  </si>
+  <si>
     <t>Ferny_Ranching.label</t>
   </si>
   <si>
-    <t>Ranching</t>
+    <t>Influence</t>
   </si>
   <si>
     <r>
@@ -1195,9 +1195,6 @@
     <t>Transport</t>
   </si>
   <si>
-    <t>DesignationCategoryDef+Ferny_Transport.description</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1210,6 +1207,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Transport.description</t>
+  </si>
+  <si>
     <t>Ferny_Transport.description</t>
   </si>
   <si>
@@ -1378,16 +1378,13 @@
     <t>Ferny_TransportInfrastructure.label</t>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_TransportInfrastructure.description</t>
+  </si>
+  <si>
     <t>Ferny_TransportInfrastructure.description</t>
   </si>
   <si>
-    <t>DesignationCategoryDef+Ferny_TransportInfrastructure.description</t>
-  </si>
-  <si>
     <t>Build transport infrastructure.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Storage.label</t>
   </si>
   <si>
     <r>
@@ -1402,6 +1399,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Storage.label</t>
+  </si>
+  <si>
     <t>Ferny_Storage.label</t>
   </si>
   <si>
@@ -1966,7 +1966,7 @@
     <t>Vanilla Nutrient Paste Expanded</t>
   </si>
   <si>
-    <t>DesignationCategoryDef+Ferny_Hacking.label</t>
+    <t>Nutrients</t>
   </si>
   <si>
     <t>영양죽</t>
@@ -2209,6 +2209,18 @@
     <t>Patches.DesignationCategoryDef+Ship.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>환경</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Ship.label</t>
   </si>
   <si>
@@ -2710,9 +2722,6 @@
     <t>2x1 marriage spot</t>
   </si>
   <si>
-    <t>2x1 결혼식 장소</t>
-  </si>
-  <si>
     <t>Patches.DesignationCategoryDef+VCHE_PipeNetworks.label</t>
   </si>
   <si>
@@ -2747,18 +2756,6 @@
   </si>
   <si>
     <t>guest patient landing spot</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>환자 손님 착륙 지점</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>Patches.DesignationCategoryDef+Hygiene.label</t>
@@ -2806,9 +2803,6 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Hacking</t>
-  </si>
-  <si>
     <t>DesignationCategoryDef+Ferny_Explosives.label</t>
   </si>
   <si>
@@ -2816,9 +2810,6 @@
   </si>
   <si>
     <t>Explosives</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Explosives.description</t>
   </si>
   <si>
     <r>
@@ -2833,13 +2824,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Explosives.description</t>
+  </si>
+  <si>
     <t>Ferny_Explosives.description</t>
   </si>
   <si>
     <t>Build explosives for your enemies.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_CombatEquipment.label</t>
   </si>
   <si>
     <r>
@@ -2854,6 +2845,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_CombatEquipment.label</t>
+  </si>
+  <si>
     <t>Ferny_CombatEquipment.label</t>
   </si>
   <si>
@@ -2881,9 +2875,6 @@
     <t>Manage combat equipment.</t>
   </si>
   <si>
-    <t>DesignationCategoryDef+Ferny_Filth.label</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -2896,13 +2887,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Filth.label</t>
+  </si>
+  <si>
     <t>Ferny_Filth.label</t>
   </si>
   <si>
     <t>Filth</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Filth.description</t>
   </si>
   <si>
     <r>
@@ -2917,13 +2908,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Filth.description</t>
+  </si>
+  <si>
     <t>Ferny_Filth.description</t>
   </si>
   <si>
     <t>Manage filth.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Terraforming.label</t>
   </si>
   <si>
     <r>
@@ -2938,13 +2929,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Terraforming.label</t>
+  </si>
+  <si>
     <t>Ferny_Terraforming.label</t>
   </si>
   <si>
     <t>Terraforming</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Terraforming.description</t>
   </si>
   <si>
     <r>
@@ -2959,13 +2950,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Terraforming.description</t>
+  </si>
+  <si>
     <t>Ferny_Terraforming.description</t>
   </si>
   <si>
     <t>Manage the area environment.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Control.label</t>
   </si>
   <si>
     <r>
@@ -2980,40 +2971,28 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Control.label</t>
+  </si>
+  <si>
     <t>Ferny_Control.label</t>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Control.description</t>
+  </si>
+  <si>
     <t>Ferny_Control.description</t>
   </si>
   <si>
-    <t>DesignationCategoryDef+Ferny_Control.description</t>
-  </si>
-  <si>
-    <t>Control pawn behavior.</t>
+    <t>DesignationCategoryDef+Ferny_Management.label</t>
   </si>
   <si>
     <t>DesignationCategoryDef+Ferny_Memorial.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>정착민의 행동을 관리합니다.</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Ferny_Memorial.label</t>
   </si>
   <si>
     <t>Memorial</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Memorial.description</t>
   </si>
   <si>
     <r>
@@ -3028,13 +3007,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Memorial.description</t>
+  </si>
+  <si>
     <t>Ferny_Memorial.description</t>
   </si>
   <si>
     <t>Things that relate to burials or memorials.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_InformationStorage.label</t>
   </si>
   <si>
     <r>
@@ -3049,13 +3028,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_InformationStorage.label</t>
+  </si>
+  <si>
     <t>Ferny_InformationStorage.label</t>
   </si>
   <si>
     <t>Information</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_InformationStorage.description</t>
   </si>
   <si>
     <r>
@@ -3070,6 +3049,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_InformationStorage.description</t>
+  </si>
+  <si>
     <t>Ferny_InformationStorage.description</t>
   </si>
   <si>
@@ -3088,43 +3070,16 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
-    <t>Ferny_Hacking.label</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Logistics.label</t>
-  </si>
-  <si>
-    <t>Nutrients</t>
-  </si>
-  <si>
-    <t>Ferny_Logistics.label</t>
-  </si>
-  <si>
-    <t>Logistics</t>
+    <t>Husbandry</t>
   </si>
   <si>
     <t>DesignationCategoryDef+Ferny_VehicleStorage.label</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-      </rPr>
-      <t>물류</t>
-    </r>
-    <phoneticPr fontId="0" type="noConversion"/>
-  </si>
-  <si>
     <t>Ferny_VehicleStorage.label</t>
   </si>
   <si>
     <t>Vehicle</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_VehicleStorage.description</t>
   </si>
   <si>
     <r>
@@ -3139,13 +3094,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_VehicleStorage.description</t>
+  </si>
+  <si>
     <t>Ferny_VehicleStorage.description</t>
   </si>
   <si>
     <t>Build vehicle storage.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Summon.label</t>
   </si>
   <si>
     <r>
@@ -3160,13 +3115,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Summon.label</t>
+  </si>
+  <si>
     <t>Ferny_Summon.label</t>
   </si>
   <si>
     <t>Summon</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Summon.description</t>
   </si>
   <si>
     <r>
@@ -3181,10 +3136,10 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Summon.description</t>
+  </si>
+  <si>
     <t>Ferny_Summon.description</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_LuciferiumNetwork.label</t>
   </si>
   <si>
     <r>
@@ -3199,6 +3154,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_LuciferiumNetwork.label</t>
+  </si>
+  <si>
     <t>Ferny_LuciferiumNetwork.label</t>
   </si>
   <si>
@@ -3206,9 +3164,6 @@
   </si>
   <si>
     <t>Luciferium</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_LuciferiumNetwork.description</t>
   </si>
   <si>
     <r>
@@ -3223,13 +3178,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_LuciferiumNetwork.description</t>
+  </si>
+  <si>
     <t>Ferny_LuciferiumNetwork.description</t>
   </si>
   <si>
     <t>Manage luciferium.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_UraniumNetwork.label</t>
   </si>
   <si>
     <r>
@@ -3244,6 +3199,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_UraniumNetwork.label</t>
+  </si>
+  <si>
     <t>Ferny_UraniumNetwork.label</t>
   </si>
   <si>
@@ -3251,9 +3209,6 @@
   </si>
   <si>
     <t>Uranium</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_UraniumNetwork.description</t>
   </si>
   <si>
     <r>
@@ -3268,13 +3223,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_UraniumNetwork.description</t>
+  </si>
+  <si>
     <t>Ferny_UraniumNetwork.description</t>
   </si>
   <si>
     <t>Manage uranium.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_ToxicWasteNetwork.label</t>
   </si>
   <si>
     <r>
@@ -3289,6 +3244,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_ToxicWasteNetwork.label</t>
+  </si>
+  <si>
     <t>Ferny_ToxicWasteNetwork.label</t>
   </si>
   <si>
@@ -3296,9 +3254,6 @@
   </si>
   <si>
     <t>Toxic Waste</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_ToxicWasteNetwork.description</t>
   </si>
   <si>
     <r>
@@ -3313,13 +3268,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_ToxicWasteNetwork.description</t>
+  </si>
+  <si>
     <t>Ferny_ToxicWasteNetwork.description</t>
   </si>
   <si>
     <t>Manage toxic waste.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_DyeNetwork.label</t>
   </si>
   <si>
     <r>
@@ -3334,13 +3289,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_DyeNetwork.label</t>
+  </si>
+  <si>
     <t>Ferny_DyeNetwork.label</t>
   </si>
   <si>
     <t>Dye</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_DyeNetwork.description</t>
   </si>
   <si>
     <r>
@@ -3355,13 +3310,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_DyeNetwork.description</t>
+  </si>
+  <si>
     <t>Ferny_DyeNetwork.description</t>
   </si>
   <si>
     <t>Manage dye.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_NeutroniumNetwork.label</t>
   </si>
   <si>
     <r>
@@ -3376,6 +3331,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_NeutroniumNetwork.label</t>
+  </si>
+  <si>
     <t>Ferny_NeutroniumNetwork.label</t>
   </si>
   <si>
@@ -3383,9 +3341,6 @@
   </si>
   <si>
     <t>Neutronium</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_NeutroniumNetwork.description</t>
   </si>
   <si>
     <r>
@@ -3400,13 +3355,13 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_NeutroniumNetwork.description</t>
+  </si>
+  <si>
     <t>Ferny_NeutroniumNetwork.description</t>
   </si>
   <si>
     <t>Manage neutronium.</t>
-  </si>
-  <si>
-    <t>DesignationCategoryDef+Ferny_Hacking.description</t>
   </si>
   <si>
     <r>
@@ -3421,21 +3376,155 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>DesignationCategoryDef+Ferny_Hacking.label</t>
+  </si>
+  <si>
+    <t>Ferny_Hacking.label</t>
+  </si>
+  <si>
+    <t>Hacking</t>
+  </si>
+  <si>
+    <t>DesignationCategoryDef+Ferny_Hacking.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>해킹</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Ferny_Hacking.description</t>
   </si>
   <si>
     <t>Hack stuff.</t>
   </si>
   <si>
-    <t>해킹</t>
+    <t>Influence pawn behavior.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>해킹과 관련된 건물입니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ferny_Management.label</t>
+  </si>
+  <si>
+    <t>DesignationCategoryDef+Ferny_Management.description</t>
+  </si>
+  <si>
+    <t>Ferny_Management.description</t>
+  </si>
+  <si>
+    <t>Manage your pawns.</t>
+  </si>
+  <si>
+    <t>DesignationCategoryDef+Ferny_OxygenNetwork.label</t>
+  </si>
+  <si>
+    <t>Ferny_OxygenNetwork.label</t>
+  </si>
+  <si>
+    <t>##packageId##vanillaexpanded.gravship</t>
+  </si>
+  <si>
+    <t>Oxygen</t>
+  </si>
+  <si>
+    <t>DesignationCategoryDef+Ferny_OxygenNetwork.description</t>
+  </si>
+  <si>
+    <t>Ferny_OxygenNetwork.description</t>
+  </si>
+  <si>
+    <t>Manage oxygen.</t>
+  </si>
+  <si>
+    <t>DesignationCategoryDef+Ferny_AstrofuelNetwork.label</t>
+  </si>
+  <si>
+    <t>Ferny_AstrofuelNetwork.label</t>
+  </si>
+  <si>
+    <t>Astrofuel</t>
+  </si>
+  <si>
+    <t>DesignationCategoryDef+Ferny_AstrofuelNetwork.description</t>
+  </si>
+  <si>
+    <t>Ferny_AstrofuelNetwork.description</t>
+  </si>
+  <si>
+    <t>Manage astrofuel.</t>
+  </si>
+  <si>
+    <t>Patches.DesignationCategoryDef+UNAGI_Furniture.label</t>
+  </si>
+  <si>
+    <t>UNAGI_Furniture.label</t>
+  </si>
+  <si>
+    <t>UNAGI Decorative Furniture</t>
+  </si>
+  <si>
+    <t>UNA Decor</t>
+  </si>
+  <si>
+    <t>행동</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>관리</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>해킹과 관련된 건물입니다.</t>
+    <t>정착민을 관리합니다.</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>환경</t>
+    <t>산소</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>산소를 관리합니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>천체연료</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>천체연료를 관리합니다.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>기타 장식</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>결혼식 장소 (2x1)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>환자 도착 지점</t>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <t>정착민의 행동을 유도합니다.</t>
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
 </sst>
@@ -3795,10 +3884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F220"/>
+  <dimension ref="A1:F226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="H212" sqref="H212"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="H200" sqref="H200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -4279,18 +4368,18 @@
         <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>7</v>
@@ -4302,12 +4391,12 @@
         <v>117</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>7</v>
@@ -4384,15 +4473,15 @@
         <v>136</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>7</v>
@@ -4404,12 +4493,12 @@
         <v>140</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>7</v>
@@ -4693,29 +4782,29 @@
         <v>208</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="E53" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>7</v>
@@ -4724,7 +4813,7 @@
         <v>214</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>215</v>
+        <v>815</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>216</v>
@@ -5101,12 +5190,12 @@
         <v>303</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>7</v>
@@ -5339,29 +5428,29 @@
         <v>208</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>359</v>
       </c>
       <c r="E91" s="2" t="s">
         <v>361</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>7</v>
@@ -6130,7 +6219,7 @@
         <v>533</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>820</v>
+        <v>534</v>
       </c>
       <c r="F133" s="1" t="s">
         <v>535</v>
@@ -6267,7 +6356,7 @@
         <v>564</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.45">
@@ -6386,7 +6475,7 @@
         <v>589</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>888</v>
+        <v>591</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.45">
@@ -6397,629 +6486,629 @@
         <v>559</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A149" s="1" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A150" s="1" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A151" s="1" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A152" s="1" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A153" s="1" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A154" s="1" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A155" s="1" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A156" s="1" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A157" s="1" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A158" s="1" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="E158" s="2" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A159" s="1" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A160" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A161" s="1" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="E161" s="2" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F161" s="1" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A162" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B162" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E162" s="2" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="F162" s="1" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A163" s="1" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="B163" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="F163" s="1" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A164" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="F164" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A165" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="F165" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A166" s="1" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="F166" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A167" s="1" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="F167" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A168" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="F168" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A169" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="F169" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A170" s="1" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="B170" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="F170" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A171" s="1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F171" s="1" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A172" s="1" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="F172" s="1" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A173" s="1" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="F173" s="1" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A174" s="1" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B174" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="E174" s="2" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="F174" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A175" s="1" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B175" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="F175" s="1" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A176" s="1" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="F176" s="1" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A177" s="1" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>559</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="E177" s="2" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="F177" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A178" s="1" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>559</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>295</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="F178" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A179" s="1" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>559</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="F179" s="1" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A180" s="1" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>559</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="F180" s="1" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A181" s="1" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>559</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="F181" s="1" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A182" s="1" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>559</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="F182" s="1" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A183" s="1" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="F183" s="1" t="s">
-        <v>737</v>
+        <v>913</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.45">
@@ -7067,7 +7156,7 @@
         <v>746</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="C186" s="1" t="s">
         <v>747</v>
@@ -7079,52 +7168,52 @@
         <v>749</v>
       </c>
       <c r="F186" s="1" t="s">
-        <v>750</v>
+        <v>914</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A187" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>559</v>
       </c>
       <c r="C187" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="D187" s="1" t="s">
         <v>752</v>
       </c>
-      <c r="D187" s="1" t="s">
+      <c r="E187" s="2" t="s">
         <v>753</v>
       </c>
-      <c r="E187" s="2" t="s">
+      <c r="F187" s="1" t="s">
         <v>754</v>
-      </c>
-      <c r="F187" s="1" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A188" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>559</v>
       </c>
       <c r="C188" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D188" s="1" t="s">
         <v>757</v>
       </c>
-      <c r="D188" s="1" t="s">
+      <c r="E188" s="2" t="s">
         <v>758</v>
       </c>
-      <c r="E188" s="2" t="s">
+      <c r="F188" s="1" t="s">
         <v>759</v>
-      </c>
-      <c r="F188" s="1" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A189" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>7</v>
@@ -7139,552 +7228,552 @@
         <v>740</v>
       </c>
       <c r="F189" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A190" s="1" t="s">
+        <v>762</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="E190" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="B190" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C190" s="1" t="s">
+      <c r="F190" s="1" t="s">
         <v>765</v>
-      </c>
-      <c r="E190" s="2" t="s">
-        <v>766</v>
-      </c>
-      <c r="F190" s="1" t="s">
-        <v>768</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A191" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C191" s="1" t="s">
         <v>767</v>
       </c>
-      <c r="B191" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C191" s="1" t="s">
+      <c r="E191" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="F191" s="1" t="s">
         <v>769</v>
-      </c>
-      <c r="E191" s="2" t="s">
-        <v>770</v>
-      </c>
-      <c r="F191" s="1" t="s">
-        <v>772</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A192" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C192" s="1" t="s">
         <v>771</v>
       </c>
-      <c r="B192" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C192" s="1" t="s">
+      <c r="E192" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="F192" s="1" t="s">
         <v>773</v>
-      </c>
-      <c r="E192" s="2" t="s">
-        <v>774</v>
-      </c>
-      <c r="F192" s="1" t="s">
-        <v>775</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A193" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="E193" s="2" t="s">
         <v>776</v>
       </c>
-      <c r="B193" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C193" s="1" t="s">
+      <c r="F193" s="1" t="s">
         <v>777</v>
-      </c>
-      <c r="E193" s="2" t="s">
-        <v>778</v>
-      </c>
-      <c r="F193" s="1" t="s">
-        <v>780</v>
       </c>
     </row>
     <row r="194" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A194" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C194" s="1" t="s">
         <v>779</v>
       </c>
-      <c r="B194" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C194" s="1" t="s">
+      <c r="E194" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="F194" s="1" t="s">
         <v>781</v>
-      </c>
-      <c r="E194" s="2" t="s">
-        <v>782</v>
-      </c>
-      <c r="F194" s="1" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A195" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C195" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="B195" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C195" s="1" t="s">
+      <c r="E195" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="F195" s="1" t="s">
         <v>785</v>
-      </c>
-      <c r="E195" s="2" t="s">
-        <v>786</v>
-      </c>
-      <c r="F195" s="1" t="s">
-        <v>788</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A196" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C196" s="1" t="s">
         <v>787</v>
       </c>
-      <c r="B196" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C196" s="1" t="s">
+      <c r="E196" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="F196" s="1" t="s">
         <v>789</v>
-      </c>
-      <c r="E196" s="2" t="s">
-        <v>790</v>
-      </c>
-      <c r="F196" s="1" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A197" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C197" s="1" t="s">
         <v>791</v>
       </c>
-      <c r="B197" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C197" s="1" t="s">
+      <c r="E197" s="2" t="s">
+        <v>792</v>
+      </c>
+      <c r="F197" s="1" t="s">
         <v>793</v>
-      </c>
-      <c r="E197" s="2" t="s">
-        <v>794</v>
-      </c>
-      <c r="F197" s="1" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A198" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C198" s="1" t="s">
         <v>795</v>
       </c>
-      <c r="B198" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C198" s="1" t="s">
-        <v>797</v>
-      </c>
       <c r="E198" s="2" t="s">
-        <v>564</v>
+        <v>215</v>
       </c>
       <c r="F198" s="1" t="s">
-        <v>115</v>
+        <v>905</v>
       </c>
     </row>
     <row r="199" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A199" s="1" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="E199" s="2" t="s">
-        <v>800</v>
+        <v>882</v>
       </c>
       <c r="F199" s="1" t="s">
-        <v>802</v>
+        <v>915</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A200" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="E200" s="2" t="s">
         <v>801</v>
       </c>
-      <c r="B200" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C200" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="E200" s="2" t="s">
-        <v>804</v>
-      </c>
       <c r="F200" s="1" t="s">
-        <v>806</v>
+        <v>802</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A201" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="E201" s="2" t="s">
         <v>805</v>
       </c>
-      <c r="B201" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C201" s="1" t="s">
-        <v>807</v>
-      </c>
-      <c r="E201" s="2" t="s">
-        <v>808</v>
-      </c>
       <c r="F201" s="1" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A202" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="E202" s="2" t="s">
         <v>809</v>
       </c>
-      <c r="B202" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C202" s="1" t="s">
-        <v>811</v>
-      </c>
-      <c r="E202" s="2" t="s">
-        <v>812</v>
-      </c>
       <c r="F202" s="1" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
     </row>
     <row r="203" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A203" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="E203" s="2" t="s">
         <v>813</v>
       </c>
-      <c r="B203" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C203" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="E203" s="2" t="s">
-        <v>816</v>
-      </c>
       <c r="F203" s="1" t="s">
-        <v>817</v>
+        <v>814</v>
       </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A204" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>817</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>818</v>
+      </c>
+      <c r="F204" s="1" t="s">
         <v>819</v>
-      </c>
-      <c r="B204" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C204" s="1" t="s">
-        <v>821</v>
-      </c>
-      <c r="E204" s="2" t="s">
-        <v>822</v>
-      </c>
-      <c r="F204" s="1" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="205" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A205" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C205" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="E205" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="F205" s="1" t="s">
         <v>823</v>
-      </c>
-      <c r="B205" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>825</v>
-      </c>
-      <c r="E205" s="2" t="s">
-        <v>826</v>
-      </c>
-      <c r="F205" s="1" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A206" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="B206" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C206" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="E206" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="F206" s="1" t="s">
         <v>827</v>
-      </c>
-      <c r="B206" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C206" s="1" t="s">
-        <v>829</v>
-      </c>
-      <c r="E206" s="2" t="s">
-        <v>830</v>
-      </c>
-      <c r="F206" s="1" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A207" s="1" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>833</v>
+        <v>829</v>
       </c>
       <c r="E207" s="2" t="s">
-        <v>834</v>
+        <v>423</v>
       </c>
       <c r="F207" s="1" t="s">
-        <v>836</v>
+        <v>830</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A208" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="B208" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C208" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="D208" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="E208" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="F208" s="1" t="s">
         <v>835</v>
-      </c>
-      <c r="B208" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C208" s="1" t="s">
-        <v>837</v>
-      </c>
-      <c r="E208" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="F208" s="1" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A209" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C209" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="D209" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="E209" s="2" t="s">
         <v>838</v>
       </c>
-      <c r="B209" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C209" s="1" t="s">
-        <v>840</v>
-      </c>
-      <c r="D209" s="1" t="s">
-        <v>841</v>
-      </c>
-      <c r="E209" s="2" t="s">
-        <v>842</v>
-      </c>
       <c r="F209" s="1" t="s">
-        <v>844</v>
+        <v>839</v>
       </c>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A210" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="B210" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C210" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="D210" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="E210" s="2" t="s">
         <v>843</v>
       </c>
-      <c r="B210" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C210" s="1" t="s">
-        <v>845</v>
-      </c>
-      <c r="D210" s="1" t="s">
-        <v>841</v>
-      </c>
-      <c r="E210" s="2" t="s">
-        <v>846</v>
-      </c>
       <c r="F210" s="1" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A211" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C211" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="D211" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="E211" s="2" t="s">
         <v>847</v>
       </c>
-      <c r="B211" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C211" s="1" t="s">
-        <v>849</v>
-      </c>
-      <c r="D211" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="E211" s="2" t="s">
-        <v>851</v>
-      </c>
       <c r="F211" s="1" t="s">
-        <v>853</v>
+        <v>848</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A212" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="B212" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C212" s="1" t="s">
+        <v>850</v>
+      </c>
+      <c r="D212" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="E212" s="2" t="s">
         <v>852</v>
       </c>
-      <c r="B212" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C212" s="1" t="s">
-        <v>854</v>
-      </c>
-      <c r="D212" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="E212" s="2" t="s">
-        <v>855</v>
-      </c>
       <c r="F212" s="1" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A213" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="D213" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="E213" s="2" t="s">
         <v>856</v>
       </c>
-      <c r="B213" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C213" s="1" t="s">
-        <v>858</v>
-      </c>
-      <c r="D213" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="E213" s="2" t="s">
-        <v>860</v>
-      </c>
       <c r="F213" s="1" t="s">
-        <v>862</v>
+        <v>857</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A214" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="E214" s="2" t="s">
+        <v>860</v>
+      </c>
+      <c r="F214" s="1" t="s">
         <v>861</v>
-      </c>
-      <c r="B214" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C214" s="1" t="s">
-        <v>863</v>
-      </c>
-      <c r="D214" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="E214" s="2" t="s">
-        <v>864</v>
-      </c>
-      <c r="F214" s="1" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A215" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="D215" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="E215" s="2" t="s">
+        <v>864</v>
+      </c>
+      <c r="F215" s="1" t="s">
         <v>865</v>
-      </c>
-      <c r="B215" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C215" s="1" t="s">
-        <v>867</v>
-      </c>
-      <c r="D215" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="E215" s="2" t="s">
-        <v>868</v>
-      </c>
-      <c r="F215" s="1" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A216" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B216" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="D216" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="E216" s="2" t="s">
         <v>869</v>
       </c>
-      <c r="B216" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C216" s="1" t="s">
-        <v>871</v>
-      </c>
-      <c r="D216" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="E216" s="2" t="s">
-        <v>872</v>
-      </c>
       <c r="F216" s="1" t="s">
-        <v>874</v>
+        <v>870</v>
       </c>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A217" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="D217" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="E217" s="2" t="s">
         <v>873</v>
       </c>
-      <c r="B217" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C217" s="1" t="s">
-        <v>875</v>
-      </c>
-      <c r="D217" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="E217" s="2" t="s">
-        <v>877</v>
-      </c>
       <c r="F217" s="1" t="s">
-        <v>879</v>
+        <v>874</v>
       </c>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A218" s="1" t="s">
-        <v>878</v>
+        <v>875</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>880</v>
-      </c>
-      <c r="D218" s="1" t="s">
         <v>876</v>
       </c>
       <c r="E218" s="2" t="s">
-        <v>881</v>
+        <v>877</v>
       </c>
       <c r="F218" s="1" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A219" s="1" t="s">
-        <v>534</v>
+        <v>878</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>818</v>
+        <v>880</v>
       </c>
       <c r="E219" s="2" t="s">
-        <v>763</v>
+        <v>881</v>
       </c>
       <c r="F219" s="1" t="s">
-        <v>886</v>
+        <v>883</v>
       </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A220" s="1" t="s">
-        <v>882</v>
+        <v>798</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>7</v>
@@ -7693,10 +7782,127 @@
         <v>884</v>
       </c>
       <c r="E220" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="F220" s="1" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A221" s="1" t="s">
         <v>885</v>
       </c>
-      <c r="F220" s="1" t="s">
+      <c r="B221" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C221" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="E221" s="2" t="s">
         <v>887</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A222" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="B222" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C222" s="1" t="s">
+        <v>889</v>
+      </c>
+      <c r="D222" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="E222" s="2" t="s">
+        <v>891</v>
+      </c>
+      <c r="F222" s="1" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A223" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C223" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="D223" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="E223" s="2" t="s">
+        <v>894</v>
+      </c>
+      <c r="F223" s="1" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A224" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="B224" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C224" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="D224" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="E224" s="2" t="s">
+        <v>897</v>
+      </c>
+      <c r="F224" s="1" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A225" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C225" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="D225" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="E225" s="2" t="s">
+        <v>900</v>
+      </c>
+      <c r="F225" s="1" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A226" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="B226" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C226" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="D226" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="E226" s="2" t="s">
+        <v>904</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>912</v>
       </c>
     </row>
   </sheetData>

</xml_diff>